<commit_message>
Update goxcel handlers and excel package
</commit_message>
<xml_diff>
--- a/gastos_ingresos_template.xlsx
+++ b/gastos_ingresos_template.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DD7E4C4-9395-4790-ACE6-C29B056EBF9B}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\henrr\mine\goxcel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB3A727-197B-46DE-B75F-47421D366D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meses" sheetId="1" r:id="rId1"/>
-    <sheet name="Semanas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>Enero</t>
   </si>
@@ -75,12 +79,18 @@
   <si>
     <t>Ingresos</t>
   </si>
+  <si>
+    <t>Día 1 del mes</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,15 +99,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -105,12 +133,173 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,9 +318,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +358,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -275,7 +464,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -417,7 +606,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -425,141 +614,1051 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" s="1"/>
+      <c r="K1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1" s="6"/>
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="P1" s="1"/>
+      <c r="Q1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
+      <c r="R1" s="6"/>
+      <c r="S1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U1" t="s">
+      <c r="T1" s="1"/>
+      <c r="U1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="W1" t="s">
+      <c r="V1" s="6"/>
+      <c r="W1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" t="s">
+      <c r="X1" s="3"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="15" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="17"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="17"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="17"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="17"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="17"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="17"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="17"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="17"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="17"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="17"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="17"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="17"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="17"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="17"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="16"/>
+      <c r="X18" s="17"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="16"/>
+      <c r="X19" s="17"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="17"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="16"/>
+      <c r="X21" s="17"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="17"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="17"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="17"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="17"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="17"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="17"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="16"/>
+      <c r="X28" s="17"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="17"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="16"/>
+      <c r="X30" s="17"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
+      <c r="B31" s="2"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="16"/>
+      <c r="X31" s="17"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
+      <c r="B32" s="2"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="20"/>
+      <c r="W32" s="16"/>
+      <c r="X32" s="17"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="18"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="18"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="18"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="18"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="11"/>
+      <c r="W33" s="12"/>
+      <c r="X33" s="18"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f>SUM(A3:A33)</f>
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <f>SUM(B3:B33)</f>
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f>SUM(C3:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f>SUM(D3:D30)</f>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f>SUM(E3:E33)</f>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f>SUM(F3:F32)</f>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f>SUM(G3:G32)</f>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f>SUM(H3:H32)</f>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f>SUM(I3:I33)</f>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f>SUM(J3:J33)</f>
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f>SUM(K3:K32)</f>
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <f>SUM(L3:L32)</f>
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f>SUM(M3:M33)</f>
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ref="B34:X34" si="0">SUM(N3:N33)</f>
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <f>SUM(Q3:Q32)</f>
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <f>SUM(R3:R32)</f>
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <f>SUM(S3:S33)</f>
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <f>SUM(U3:U32)</f>
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <f>SUM(V3:V32)</f>
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1242BF18-061A-41FF-846F-23E25D256E8F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <mergeCells count="12">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="M1:N1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>